<commit_message>
With style for number
</commit_message>
<xml_diff>
--- a/tests/Resources/Doubles.xlsx
+++ b/tests/Resources/Doubles.xlsx
@@ -27,7 +27,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,6 +38,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -69,27 +75,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -394,52 +391,32 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="17.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>2.2345</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>